<commit_message>
changes to guo nian li
</commit_message>
<xml_diff>
--- a/ceremonies/過年禮.xlsx
+++ b/ceremonies/過年禮.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Xepht\Documents\Xepht\Scripts\Temple\phonetic guide\ceremonies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA375C2E-7762-4614-B268-46E82DF31633}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC20E6D-5317-4BA5-8DC0-F50E6B0B95A9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{599E5732-C87C-4C4D-AC6C-0C4EE14224B7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{599E5732-C87C-4C4D-AC6C-0C4EE14224B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -519,12 +519,6 @@
     <t>bài nián</t>
   </si>
   <si>
-    <t>向明明上帝祝壽</t>
-  </si>
-  <si>
-    <t>xiàng míng míng shàng dì zhù shòu</t>
-  </si>
-  <si>
     <t>zuò yī hòu èr wèi guì</t>
   </si>
   <si>
@@ -768,9 +762,6 @@
     <t>ㄐㄧㄡˇ ㄎㄡ` ㄕㄡˇ</t>
   </si>
   <si>
-    <t>ㄒㄧㄤ` ㄇㄧㄥˊ ㄇㄧㄥˊ ㄕㄤ` ㄉㄧ` ㄓㄨ` ㄕㄡ`</t>
-  </si>
-  <si>
     <t>ㄧˇ ㄒㄧㄚ` ㄍㄜ` ㄗ` ㄍㄨㄟ ㄨㄟ`</t>
   </si>
   <si>
@@ -790,6 +781,15 @@
   </si>
   <si>
     <t>break</t>
+  </si>
+  <si>
+    <t>向彌勒祖師祝壽</t>
+  </si>
+  <si>
+    <t>xiàng mí lè zǔ shī zhù shòu</t>
+  </si>
+  <si>
+    <t>ㄒㄧㄤ` ㄇㄧˊ ㄌㄜ` ㄗㄨˇ ㄕ ㄓㄨ` ㄕㄡ`</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F35F471-445B-4871-B79C-3B7C0D3FB683}">
-  <dimension ref="A1:E313"/>
+  <dimension ref="A1:E319"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
+    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="D320" sqref="D320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1171,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
         <v>48</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1205,7 +1205,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,7 +1290,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,7 +1307,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1324,7 +1324,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,7 +1341,7 @@
         <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1372,10 +1372,10 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1409,7 +1409,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1426,7 +1426,7 @@
         <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>30</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1460,7 +1460,7 @@
         <v>28</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,10 +1474,10 @@
         <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1511,7 +1511,7 @@
         <v>28</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,7 +1545,7 @@
         <v>35</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1559,10 +1559,10 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>33</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,7 +1596,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
         <v>28</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1647,7 +1647,7 @@
         <v>28</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1661,10 +1661,10 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1681,7 +1681,7 @@
         <v>30</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1698,7 +1698,7 @@
         <v>28</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
         <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
         <v>37</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,10 +1746,10 @@
         <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,7 +1766,7 @@
         <v>33</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
         <v>27</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1800,7 +1800,7 @@
         <v>28</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>30</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v>28</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,10 +1848,10 @@
         <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1868,7 +1868,7 @@
         <v>30</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
         <v>28</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1902,7 +1902,7 @@
         <v>33</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>39</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,10 +1933,10 @@
         <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,7 +1953,7 @@
         <v>33</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>27</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>28</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>30</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,7 +2021,7 @@
         <v>28</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2035,10 +2035,10 @@
         <v>31</v>
       </c>
       <c r="D52" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>30</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,7 +2072,7 @@
         <v>28</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>33</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2106,7 +2106,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2120,10 +2120,10 @@
         <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,7 +2140,7 @@
         <v>14</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2157,7 +2157,7 @@
         <v>43</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2174,7 +2174,7 @@
         <v>45</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>7</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2208,7 +2208,7 @@
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
         <v>21</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2239,15 +2239,15 @@
         <v>46</v>
       </c>
       <c r="D64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -2265,7 +2265,7 @@
         <v>7</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>108</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2299,7 +2299,7 @@
         <v>54</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2316,7 +2316,7 @@
         <v>106</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2333,7 +2333,7 @@
         <v>50</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>56</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>106</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>52</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2401,7 +2401,7 @@
         <v>58</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>106</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2435,7 +2435,7 @@
         <v>52</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,7 +2452,7 @@
         <v>60</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2469,7 +2469,7 @@
         <v>106</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,7 +2486,7 @@
         <v>14</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>62</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2520,7 +2520,7 @@
         <v>106</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,7 +2537,7 @@
         <v>14</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>64</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2571,7 +2571,7 @@
         <v>106</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2588,7 +2588,7 @@
         <v>14</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2605,7 +2605,7 @@
         <v>66</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2622,7 +2622,7 @@
         <v>106</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>14</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
         <v>68</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,7 +2673,7 @@
         <v>106</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
         <v>33</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2707,7 +2707,7 @@
         <v>70</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2724,7 +2724,7 @@
         <v>106</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2741,7 +2741,7 @@
         <v>33</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2758,7 +2758,7 @@
         <v>72</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2775,7 +2775,7 @@
         <v>106</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
         <v>33</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>74</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2826,7 +2826,7 @@
         <v>106</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2843,7 +2843,7 @@
         <v>33</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2860,7 +2860,7 @@
         <v>76</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -2877,7 +2877,7 @@
         <v>106</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -2894,7 +2894,7 @@
         <v>33</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -2911,7 +2911,7 @@
         <v>78</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>106</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2945,7 +2945,7 @@
         <v>33</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2962,7 +2962,7 @@
         <v>80</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -2979,7 +2979,7 @@
         <v>106</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -2996,7 +2996,7 @@
         <v>33</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -3013,7 +3013,7 @@
         <v>82</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -3030,7 +3030,7 @@
         <v>106</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>33</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -3064,7 +3064,7 @@
         <v>84</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,7 +3081,7 @@
         <v>106</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3098,7 +3098,7 @@
         <v>33</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3115,7 +3115,7 @@
         <v>86</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>106</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3149,7 +3149,7 @@
         <v>33</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3166,7 +3166,7 @@
         <v>88</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -3183,7 +3183,7 @@
         <v>106</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>33</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3217,7 +3217,7 @@
         <v>90</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3234,7 +3234,7 @@
         <v>106</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>33</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>92</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>106</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3302,7 +3302,7 @@
         <v>33</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3319,7 +3319,7 @@
         <v>94</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3336,7 +3336,7 @@
         <v>106</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3353,7 +3353,7 @@
         <v>52</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>96</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3387,7 +3387,7 @@
         <v>106</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3404,7 +3404,7 @@
         <v>52</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3421,7 +3421,7 @@
         <v>98</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3438,7 +3438,7 @@
         <v>106</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>52</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3472,7 +3472,7 @@
         <v>100</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
         <v>106</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3506,7 +3506,7 @@
         <v>14</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
         <v>102</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3540,7 +3540,7 @@
         <v>106</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3557,7 +3557,7 @@
         <v>14</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -3574,7 +3574,7 @@
         <v>104</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -3591,7 +3591,7 @@
         <v>106</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -3608,7 +3608,7 @@
         <v>14</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -3625,7 +3625,7 @@
         <v>21</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -3642,12 +3642,12 @@
         <v>110</v>
       </c>
       <c r="E147" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C148" s="1"/>
     </row>
@@ -3665,7 +3665,7 @@
         <v>7</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -3682,7 +3682,7 @@
         <v>112</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,7 +3699,7 @@
         <v>50</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -3716,7 +3716,7 @@
         <v>114</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -3733,7 +3733,7 @@
         <v>116</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,7 +3750,7 @@
         <v>118</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -3761,13 +3761,13 @@
         <v>5</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D155" t="s">
         <v>119</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -3784,7 +3784,7 @@
         <v>121</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -3801,7 +3801,7 @@
         <v>21</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,12 +3818,12 @@
         <v>123</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C159" s="1"/>
     </row>
@@ -3841,7 +3841,7 @@
         <v>125</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
@@ -3858,7 +3858,7 @@
         <v>7</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>112</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>50</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>127</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -3926,7 +3926,7 @@
         <v>129</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -3943,7 +3943,7 @@
         <v>131</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -3960,7 +3960,7 @@
         <v>133</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -3977,7 +3977,7 @@
         <v>135</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -3994,7 +3994,7 @@
         <v>137</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -4011,7 +4011,7 @@
         <v>139</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -4028,7 +4028,7 @@
         <v>141</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
         <v>143</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
@@ -4062,7 +4062,7 @@
         <v>145</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
@@ -4079,7 +4079,7 @@
         <v>7</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
@@ -4096,7 +4096,7 @@
         <v>147</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
@@ -4113,7 +4113,7 @@
         <v>14</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
@@ -4130,7 +4130,7 @@
         <v>149</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
@@ -4147,7 +4147,7 @@
         <v>151</v>
       </c>
       <c r="E178" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
@@ -4164,7 +4164,7 @@
         <v>14</v>
       </c>
       <c r="E179" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
@@ -4181,7 +4181,7 @@
         <v>149</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
@@ -4198,7 +4198,7 @@
         <v>153</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
@@ -4215,7 +4215,7 @@
         <v>14</v>
       </c>
       <c r="E182" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
@@ -4229,10 +4229,10 @@
         <v>154</v>
       </c>
       <c r="D183" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
@@ -4249,7 +4249,7 @@
         <v>112</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>52</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
@@ -4280,10 +4280,10 @@
         <v>154</v>
       </c>
       <c r="D186" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
         <v>112</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -4317,7 +4317,7 @@
         <v>54</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
@@ -4334,7 +4334,7 @@
         <v>161</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
@@ -4351,7 +4351,7 @@
         <v>50</v>
       </c>
       <c r="E190" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
@@ -4365,10 +4365,10 @@
         <v>154</v>
       </c>
       <c r="D191" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E191" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
@@ -4385,7 +4385,7 @@
         <v>11</v>
       </c>
       <c r="E192" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -4402,7 +4402,7 @@
         <v>56</v>
       </c>
       <c r="E193" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4419,7 +4419,7 @@
         <v>161</v>
       </c>
       <c r="E194" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4436,7 +4436,7 @@
         <v>156</v>
       </c>
       <c r="E195" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4450,10 +4450,10 @@
         <v>154</v>
       </c>
       <c r="D196" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E196" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>11</v>
       </c>
       <c r="E197" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4487,7 +4487,7 @@
         <v>58</v>
       </c>
       <c r="E198" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4504,7 +4504,7 @@
         <v>161</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4521,7 +4521,7 @@
         <v>156</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4535,10 +4535,10 @@
         <v>154</v>
       </c>
       <c r="D201" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E201" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4555,7 +4555,7 @@
         <v>11</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4572,7 +4572,7 @@
         <v>60</v>
       </c>
       <c r="E203" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -4589,7 +4589,7 @@
         <v>161</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -4606,7 +4606,7 @@
         <v>52</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -4623,7 +4623,7 @@
         <v>11</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -4640,7 +4640,7 @@
         <v>62</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -4657,7 +4657,7 @@
         <v>161</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -4674,7 +4674,7 @@
         <v>52</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -4691,7 +4691,7 @@
         <v>11</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -4708,7 +4708,7 @@
         <v>64</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -4725,7 +4725,7 @@
         <v>161</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -4742,7 +4742,7 @@
         <v>52</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -4759,7 +4759,7 @@
         <v>11</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -4776,7 +4776,7 @@
         <v>66</v>
       </c>
       <c r="E215" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
@@ -4793,7 +4793,7 @@
         <v>161</v>
       </c>
       <c r="E216" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -4810,7 +4810,7 @@
         <v>52</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -4827,7 +4827,7 @@
         <v>11</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>68</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -4861,7 +4861,7 @@
         <v>161</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -4878,7 +4878,7 @@
         <v>14</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -4895,7 +4895,7 @@
         <v>70</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -4912,7 +4912,7 @@
         <v>161</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">
@@ -4929,7 +4929,7 @@
         <v>14</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
@@ -4946,7 +4946,7 @@
         <v>72</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.25">
@@ -4963,7 +4963,7 @@
         <v>161</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
@@ -4980,7 +4980,7 @@
         <v>14</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.25">
@@ -4997,7 +4997,7 @@
         <v>11</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
@@ -5014,7 +5014,7 @@
         <v>74</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>161</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
@@ -5048,7 +5048,7 @@
         <v>14</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.25">
@@ -5065,7 +5065,7 @@
         <v>76</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
@@ -5082,7 +5082,7 @@
         <v>161</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.25">
@@ -5099,7 +5099,7 @@
         <v>14</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
@@ -5116,7 +5116,7 @@
         <v>78</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.25">
@@ -5133,7 +5133,7 @@
         <v>161</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
@@ -5150,7 +5150,7 @@
         <v>14</v>
       </c>
       <c r="E237" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.25">
@@ -5167,7 +5167,7 @@
         <v>11</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
@@ -5184,7 +5184,7 @@
         <v>80</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.25">
@@ -5201,7 +5201,7 @@
         <v>161</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5218,7 +5218,7 @@
         <v>14</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.25">
@@ -5235,7 +5235,7 @@
         <v>82</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
@@ -5252,7 +5252,7 @@
         <v>161</v>
       </c>
       <c r="E243" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.25">
@@ -5269,7 +5269,7 @@
         <v>33</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
@@ -5286,7 +5286,7 @@
         <v>84</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.25">
@@ -5303,7 +5303,7 @@
         <v>161</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
@@ -5320,7 +5320,7 @@
         <v>33</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.25">
@@ -5337,7 +5337,7 @@
         <v>86</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
@@ -5354,7 +5354,7 @@
         <v>161</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.25">
@@ -5371,7 +5371,7 @@
         <v>33</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
@@ -5388,7 +5388,7 @@
         <v>88</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.25">
@@ -5405,7 +5405,7 @@
         <v>161</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
@@ -5422,7 +5422,7 @@
         <v>33</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.25">
@@ -5439,7 +5439,7 @@
         <v>90</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
@@ -5456,7 +5456,7 @@
         <v>161</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.25">
@@ -5473,7 +5473,7 @@
         <v>33</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -5490,7 +5490,7 @@
         <v>92</v>
       </c>
       <c r="E257" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
@@ -5507,7 +5507,7 @@
         <v>161</v>
       </c>
       <c r="E258" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
@@ -5524,7 +5524,7 @@
         <v>33</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
@@ -5538,10 +5538,10 @@
         <v>154</v>
       </c>
       <c r="D260" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
@@ -5558,7 +5558,7 @@
         <v>11</v>
       </c>
       <c r="E261" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
@@ -5575,7 +5575,7 @@
         <v>94</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
@@ -5592,7 +5592,7 @@
         <v>161</v>
       </c>
       <c r="E263" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
@@ -5609,7 +5609,7 @@
         <v>52</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
@@ -5626,7 +5626,7 @@
         <v>11</v>
       </c>
       <c r="E265" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
@@ -5643,7 +5643,7 @@
         <v>96</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
@@ -5660,7 +5660,7 @@
         <v>161</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -5677,7 +5677,7 @@
         <v>52</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -5694,7 +5694,7 @@
         <v>11</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
@@ -5711,7 +5711,7 @@
         <v>98</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -5728,7 +5728,7 @@
         <v>161</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
@@ -5745,7 +5745,7 @@
         <v>52</v>
       </c>
       <c r="E272" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -5762,7 +5762,7 @@
         <v>11</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
@@ -5779,7 +5779,7 @@
         <v>100</v>
       </c>
       <c r="E274" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
@@ -5796,7 +5796,7 @@
         <v>161</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
@@ -5813,7 +5813,7 @@
         <v>14</v>
       </c>
       <c r="E276" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -5830,7 +5830,7 @@
         <v>11</v>
       </c>
       <c r="E277" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -5847,7 +5847,7 @@
         <v>102</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
@@ -5864,7 +5864,7 @@
         <v>161</v>
       </c>
       <c r="E279" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
@@ -5881,7 +5881,7 @@
         <v>14</v>
       </c>
       <c r="E280" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
@@ -5898,7 +5898,7 @@
         <v>11</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
@@ -5915,7 +5915,7 @@
         <v>104</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
@@ -5932,7 +5932,7 @@
         <v>161</v>
       </c>
       <c r="E283" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
@@ -5949,7 +5949,7 @@
         <v>14</v>
       </c>
       <c r="E284" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
@@ -5963,10 +5963,10 @@
         <v>154</v>
       </c>
       <c r="D285" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E285" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
@@ -5977,13 +5977,13 @@
         <v>15</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>162</v>
+        <v>250</v>
       </c>
       <c r="D286" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
       <c r="E286" s="1" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
@@ -6000,7 +6000,7 @@
         <v>147</v>
       </c>
       <c r="E287" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
@@ -6017,7 +6017,7 @@
         <v>14</v>
       </c>
       <c r="E288" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
@@ -6034,7 +6034,7 @@
         <v>149</v>
       </c>
       <c r="E289" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -6051,7 +6051,7 @@
         <v>151</v>
       </c>
       <c r="E290" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -6068,7 +6068,7 @@
         <v>14</v>
       </c>
       <c r="E291" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
@@ -6085,7 +6085,7 @@
         <v>149</v>
       </c>
       <c r="E292" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -6102,7 +6102,7 @@
         <v>153</v>
       </c>
       <c r="E293" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -6119,7 +6119,7 @@
         <v>14</v>
       </c>
       <c r="E294" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -6136,7 +6136,7 @@
         <v>127</v>
       </c>
       <c r="E295" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -6153,7 +6153,7 @@
         <v>133</v>
       </c>
       <c r="E296" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="297" spans="1:5" x14ac:dyDescent="0.25">
@@ -6170,7 +6170,7 @@
         <v>135</v>
       </c>
       <c r="E297" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -6187,7 +6187,7 @@
         <v>137</v>
       </c>
       <c r="E298" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
@@ -6204,7 +6204,7 @@
         <v>139</v>
       </c>
       <c r="E299" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="300" spans="1:5" x14ac:dyDescent="0.25">
@@ -6221,7 +6221,7 @@
         <v>141</v>
       </c>
       <c r="E300" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="301" spans="1:5" x14ac:dyDescent="0.25">
@@ -6238,7 +6238,7 @@
         <v>143</v>
       </c>
       <c r="E301" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
@@ -6255,7 +6255,7 @@
         <v>158</v>
       </c>
       <c r="E302" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -6269,15 +6269,15 @@
         <v>159</v>
       </c>
       <c r="D303" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E303" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C304" s="1"/>
     </row>
@@ -6295,7 +6295,7 @@
         <v>7</v>
       </c>
       <c r="E305" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
@@ -6312,7 +6312,7 @@
         <v>112</v>
       </c>
       <c r="E306" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
@@ -6329,7 +6329,7 @@
         <v>50</v>
       </c>
       <c r="E307" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
@@ -6346,7 +6346,7 @@
         <v>116</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
@@ -6363,7 +6363,7 @@
         <v>118</v>
       </c>
       <c r="E309" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
@@ -6374,13 +6374,13 @@
         <v>5</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D310" t="s">
         <v>119</v>
       </c>
       <c r="E310" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
@@ -6397,7 +6397,7 @@
         <v>121</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -6414,7 +6414,7 @@
         <v>21</v>
       </c>
       <c r="E312" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -6425,14 +6425,17 @@
         <v>12</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="D313" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="E313" s="1" t="s">
-        <v>227</v>
-      </c>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C319" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>